<commit_message>
refactor for simple version
</commit_message>
<xml_diff>
--- a/db/model/init_sql.xlsx
+++ b/db/model/init_sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yinping/work/projects/blueberry/service_starter/db/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B870B1-B729-9740-A811-2748CE201B91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282AE0ED-D01A-E341-99D5-6495C6C7C0AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{7F77F5F8-1C91-CE46-B772-1760AFD20BD5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>删除状态</t>
   </si>
@@ -73,51 +73,6 @@
   </si>
   <si>
     <t>是否启用</t>
-  </si>
-  <si>
-    <t>APP</t>
-  </si>
-  <si>
-    <t>消息状态</t>
-  </si>
-  <si>
-    <t>收到</t>
-  </si>
-  <si>
-    <t>队列</t>
-  </si>
-  <si>
-    <t>发送</t>
-  </si>
-  <si>
-    <t>成功</t>
-  </si>
-  <si>
-    <t>取消</t>
-  </si>
-  <si>
-    <t>失败</t>
-  </si>
-  <si>
-    <t>消息大类</t>
-  </si>
-  <si>
-    <t>SMS</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>消息小类</t>
-  </si>
-  <si>
-    <t>HTML</t>
-  </si>
-  <si>
-    <t>PLAIN</t>
-  </si>
-  <si>
-    <t>邮件内容类型</t>
   </si>
 </sst>
 </file>
@@ -476,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1C2B13-3C20-0447-81A3-E11BB3A5A6D9}">
-  <dimension ref="B1:I17"/>
+  <dimension ref="B1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,306 +563,6 @@
         <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','公用', '是否启用','1008','停用', '100802',  '');</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>1020</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H17" si="2">D6*100+F6</f>
-        <v>102001</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" ref="I6:I17" si="3">CONCATENATE("INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','"&amp;B6&amp;"', '"&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"', '"&amp;H6&amp;"',  '"&amp;G6&amp;"');")</f>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息状态','1020','收到', '102001',  '');</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>1020</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
-        <v>102002</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息状态','1020','队列', '102002',  '');</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <v>1020</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
-        <v>102003</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息状态','1020','发送', '102003',  '');</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>1020</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>102004</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息状态','1020','成功', '102004',  '');</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>1020</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>102005</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息状态','1020','取消', '102005',  '');</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>1020</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>102006</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息状态','1020','失败', '102006',  '');</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
-        <v>1021</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>102101</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息大类','1021','SMS', '102101',  '');</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13">
-        <v>1021</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>102102</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息大类','1021','EMAIL', '102102',  '');</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <v>1022</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>102201</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息小类','1022','SMS', '102201',  '');</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15">
-        <v>1022</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>102202</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '消息小类','1022','EMAIL', '102202',  '');</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16">
-        <v>1023</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>102301</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '邮件内容类型','1023','HTML', '102301',  '');</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17">
-        <v>1023</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>102302</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO `dictionary`(`created_by`, `enable`,`module`, `type_name`,`type_code`, `name`,`value`,`remark`)  VALUES (-1,'100801','APP', '邮件内容类型','1023','PLAIN', '102302',  '');</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>